<commit_message>
Módulo 13 - Ferramenta de Análises (tabela de dados)
</commit_message>
<xml_diff>
--- a/Módulo 13 - Analise de dados/aula-tabela-dados.xlsx
+++ b/Módulo 13 - Analise de dados/aula-tabela-dados.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Google Drive\Curso_Excel\12 Ferramentas de análise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\Módulo 13 - Analise de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCF86A0-B42E-4BE6-98AA-BE6292050F9A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4430C8C5-1BA6-4289-86B7-BC19EE26AF37}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela de Dados 1" sheetId="2" r:id="rId1"/>
     <sheet name="Tabela de Dados 2" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Público estimado</t>
   </si>
@@ -109,11 +108,43 @@
   <si>
     <t>Preço do Ingresso</t>
   </si>
+  <si>
+    <t>Analisa vários cenários possivéis do impacto de duas variáveis em um resultado desejado</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tabela de dados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> faz a mesma coisa que o gerenciador de cenários só que de forma mais visual</t>
+    </r>
+  </si>
+  <si>
+    <t>vai dar lucro ou não, de acordo com o preço do ingresso mais público estimado?</t>
+  </si>
+  <si>
+    <t>Criar tabela: dados/teste de hipoteses/tabela de dados/célula de entrada da linha (os dados que estão posicionados na horizontal). E na célula de entrada da coluna insere o dado que está agrupado na vertical</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -390,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -493,6 +524,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -808,10 +842,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBD687A-3E64-44BC-B8CB-CC0BF0464A7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -868,7 +904,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>5</v>
@@ -877,7 +913,10 @@
         <v>6</v>
       </c>
       <c r="H7" s="20"/>
-      <c r="I7" s="18"/>
+      <c r="I7" s="18">
+        <f>F13</f>
+        <v>7470</v>
+      </c>
       <c r="J7" s="17">
         <v>100</v>
       </c>
@@ -893,14 +932,14 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="5">
         <f>C7*C8</f>
-        <v>10000</v>
+        <v>38000</v>
       </c>
       <c r="H8" s="29" t="s">
         <v>17</v>
@@ -908,9 +947,16 @@
       <c r="I8" s="16">
         <v>100</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="J8" s="19">
+        <f t="dataTable" ref="J8:L10" dt2D="1" dtr="1" r1="C7" r2="C8"/>
+        <v>-18950</v>
+      </c>
+      <c r="K8" s="19">
+        <v>-14125</v>
+      </c>
+      <c r="L8" s="19">
+        <v>-10265</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -930,9 +976,15 @@
       <c r="I9" s="16">
         <v>200</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="J9" s="19">
+        <v>-9900</v>
+      </c>
+      <c r="K9" s="19">
+        <v>-250</v>
+      </c>
+      <c r="L9" s="19">
+        <v>7470</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="4" t="s">
@@ -940,15 +992,21 @@
       </c>
       <c r="F10" s="5">
         <f>200*INT(C8/30)</f>
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="H10" s="31"/>
       <c r="I10" s="16">
         <v>300</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="J10" s="19">
+        <v>-1050</v>
+      </c>
+      <c r="K10" s="19">
+        <v>13425</v>
+      </c>
+      <c r="L10" s="19">
+        <v>25005</v>
+      </c>
     </row>
     <row r="11" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
@@ -956,7 +1014,7 @@
       </c>
       <c r="F11" s="5">
         <f>3000+(F8*1%)</f>
-        <v>3100</v>
+        <v>3380</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -965,12 +1023,15 @@
       </c>
       <c r="F12" s="5">
         <f>F8*2.5%</f>
-        <v>250</v>
+        <v>950</v>
       </c>
       <c r="H12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="24">
+        <f>LARGE(J8:L10,1)</f>
+        <v>25005</v>
+      </c>
     </row>
     <row r="13" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="7" t="s">
@@ -978,33 +1039,55 @@
       </c>
       <c r="F13" s="8">
         <f>F8-SUM(F9:F12)</f>
-        <v>-18950</v>
+        <v>7470</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+    </row>
+    <row r="21" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319CA7F-77A9-4D19-B255-A1F58F239FD6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>

</xml_diff>